<commit_message>
Arreglats diversos bugs del full de Incidencis Evlucion
</commit_message>
<xml_diff>
--- a/TFG/res/pacientData/1234/Resultats_REM-G1234.xlsx
+++ b/TFG/res/pacientData/1234/Resultats_REM-G1234.xlsx
@@ -4485,7 +4485,7 @@
         <v>137</v>
       </c>
       <c r="HH2" t="s">
-        <v>526</v>
+        <v>569</v>
       </c>
       <c r="HI2" t="s">
         <v>513</v>
@@ -4497,10 +4497,10 @@
         <v>605</v>
       </c>
       <c r="HL2" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="HM2" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="HN2" t="s">
         <v>606</v>

</xml_diff>